<commit_message>
Feat: Auto Push from python
</commit_message>
<xml_diff>
--- a/excel/Data.xlsx
+++ b/excel/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cglee/Dev/BackEnd/Python/db/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA39178-D097-9B47-97E8-33ECEE493E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC62813-99AE-9B4D-AD6A-6899C1A8FE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24000" yWindow="3820" windowWidth="36160" windowHeight="26140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -329,7 +329,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -412,7 +412,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>

</xml_diff>